<commit_message>
Update ADM BOM semiacabados
</commit_message>
<xml_diff>
--- a/_extrafiles/APROVADORES_PCP_09.08.2023.xlsx
+++ b/_extrafiles/APROVADORES_PCP_09.08.2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcsant\Documents\GitHub\engineering-SA\_extrafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268D7A53-A555-4E03-AAAF-9FB30D39229E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CA107B-7748-4381-9E2D-249C6111D6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="130">
   <si>
     <t>VWL</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Material absorsivo, fibra de vidro</t>
   </si>
   <si>
-    <t>SEBAREZE</t>
-  </si>
-  <si>
     <t>GSCM_002</t>
   </si>
   <si>
@@ -424,19 +421,16 @@
     <t>Importados</t>
   </si>
   <si>
-    <t>Atualizado conforme alinhamento com o Carlos Sousa no dia 09/08/2023.</t>
-  </si>
-  <si>
     <t>Nacional</t>
   </si>
   <si>
-    <t>Atualizado em: 09/08/2023</t>
-  </si>
-  <si>
-    <t>Nac. - OPT 2</t>
-  </si>
-  <si>
     <t>Tipo de material</t>
+  </si>
+  <si>
+    <t>Atualizado conforme alinhamento com o Carlos Sousa no dia 22/11/2023.</t>
+  </si>
+  <si>
+    <t>Atualizado em: 22/11/2023</t>
   </si>
 </sst>
 </file>
@@ -460,7 +454,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,12 +491,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -516,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -532,9 +520,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1138,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48DD2E8-F794-4FBC-9C70-3C0AF79762C8}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,15 +1135,15 @@
     <col min="2" max="2" width="29.85546875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
-    <col min="5" max="6" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -1166,19 +1151,16 @@
         <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>44</v>
       </c>
@@ -1189,472 +1171,440 @@
         <v>46</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="E13" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="E16" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="D28" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>127</v>
+        <v>76</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>